<commit_message>
stats for java updated
</commit_message>
<xml_diff>
--- a/Lab1/docs/Statistics.xlsx
+++ b/Lab1/docs/Statistics.xlsx
@@ -25,8 +25,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mike Pinto</author>
+  </authors>
+  <commentList>
+    <comment ref="G14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Pinto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Com as specs do sistema, para este valor, ocorreu memory swapping, o que prejudica bastante o tempo de execução dado o tempo de acesso ao disco</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>Linguagem</t>
   </si>
@@ -45,15 +79,12 @@
   <si>
     <t>Capacidade [MFLOPS/s]</t>
   </si>
-  <si>
-    <t>(Not enough memory)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +99,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -84,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -227,100 +271,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,16 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -352,31 +298,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -406,8 +340,8 @@
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2419351" cy="461963"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -595,7 +529,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -650,15 +584,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -667,8 +601,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6086475" y="1143001"/>
-          <a:ext cx="3038475" cy="561975"/>
+          <a:off x="6581775" y="1000126"/>
+          <a:ext cx="2085975" cy="1076324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -718,6 +652,41 @@
             <a:rPr lang="pt-PT" sz="1200" b="0" baseline="0"/>
             <a:t> Q6600@2.4Ghz</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="pt-PT" sz="1200" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Memória</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" sz="1400" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4GB DDR2 667Mhz</a:t>
+          </a:r>
           <a:endParaRPr lang="pt-PT" sz="1200" b="0"/>
         </a:p>
       </xdr:txBody>
@@ -737,8 +706,8 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2419351" cy="461963"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -926,7 +895,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -981,25 +950,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1504950</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8715375" y="3438525"/>
-          <a:ext cx="2276475" cy="561975"/>
+          <a:off x="8658225" y="3124200"/>
+          <a:ext cx="2085975" cy="1076324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1048,6 +1017,41 @@
           <a:r>
             <a:rPr lang="pt-PT" sz="1200" b="0" baseline="0"/>
             <a:t> Q6600@2.4Ghz</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="pt-PT" sz="1200" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Memória</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" sz="1400" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4GB DDR2 667Mhz</a:t>
           </a:r>
           <a:endParaRPr lang="pt-PT" sz="1200" b="0"/>
         </a:p>
@@ -1324,7 +1328,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,95 +1358,95 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>600</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>1.419</v>
       </c>
-      <c r="D2" s="10">
-        <f>(2*(B2^3)/C2)/1000000</f>
+      <c r="D2" s="7">
+        <f t="shared" ref="D2:D8" si="0">(2*(B2^3)/C2)/1000000</f>
         <v>304.43974630021143</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="4">
         <v>1000</v>
       </c>
       <c r="C3" s="4">
         <v>7.8129999999999997</v>
       </c>
-      <c r="D3" s="13">
-        <f>(2*(B3^3)/C3)/1000000</f>
+      <c r="D3" s="8">
+        <f t="shared" si="0"/>
         <v>255.9836170485089</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="4">
         <v>1400</v>
       </c>
       <c r="C4" s="4">
         <v>22.109000000000002</v>
       </c>
-      <c r="D4" s="13">
-        <f>(2*(B4^3)/C4)/1000000</f>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
         <v>248.22470487131935</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="4">
         <v>1800</v>
       </c>
       <c r="C5" s="4">
         <v>49.411999999999999</v>
       </c>
-      <c r="D5" s="13">
-        <f>(2*(B5^3)/C5)/1000000</f>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
         <v>236.05601878086296</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="4">
         <v>2200</v>
       </c>
       <c r="C6" s="4">
         <v>94.471999999999994</v>
       </c>
-      <c r="D6" s="13">
-        <f>(2*(B6^3)/C6)/1000000</f>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
         <v>225.42128884748919</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="4">
         <v>2600</v>
       </c>
       <c r="C7" s="4">
         <v>189.19900000000001</v>
       </c>
-      <c r="D7" s="13">
-        <f>(2*(B7^3)/C7)/1000000</f>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
         <v>185.79379383611962</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6">
         <v>3000</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>286.88600000000002</v>
       </c>
-      <c r="D8" s="14">
-        <f>(2*(B8^3)/C8)/1000000</f>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
         <v>188.22807665762704</v>
       </c>
     </row>
@@ -1467,69 +1471,69 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>600</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>2.0609999999999999</v>
       </c>
-      <c r="D11" s="10">
-        <f>(2*(B11^3)/C11)/1000000</f>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11:D17" si="1">(2*(B11^3)/C11)/1000000</f>
         <v>209.60698689956331</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="4">
         <v>1000</v>
       </c>
       <c r="C12" s="4">
         <v>12.817</v>
       </c>
-      <c r="D12" s="13">
-        <f>(2*(B12^3)/C12)/1000000</f>
+      <c r="D12" s="8">
+        <f t="shared" si="1"/>
         <v>156.04275571506594</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="4">
         <v>1400</v>
       </c>
       <c r="C13" s="4">
         <v>37.072000000000003</v>
       </c>
-      <c r="D13" s="13">
-        <f>(2*(B13^3)/C13)/1000000</f>
+      <c r="D13" s="8">
+        <f t="shared" si="1"/>
         <v>148.03625377643505</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="4">
         <v>1800</v>
       </c>
       <c r="C14" s="4">
         <v>86.454999999999998</v>
       </c>
-      <c r="D14" s="13">
-        <f>(2*(B14^3)/C14)/1000000</f>
+      <c r="D14" s="8">
+        <f t="shared" si="1"/>
         <v>134.91411717078248</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="4">
         <v>2200</v>
       </c>
       <c r="C15" s="4">
         <v>175.66900000000001</v>
       </c>
-      <c r="D15" s="13">
-        <f>(2*(B15^3)/C15)/1000000</f>
+      <c r="D15" s="8">
+        <f t="shared" si="1"/>
         <v>121.22799127905321</v>
       </c>
       <c r="F15" s="3"/>
@@ -1538,15 +1542,15 @@
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="4">
         <v>2600</v>
       </c>
       <c r="C16" s="4">
         <v>294.61099999999999</v>
       </c>
-      <c r="D16" s="13">
-        <f>(2*(B16^3)/C16)/1000000</f>
+      <c r="D16" s="8">
+        <f t="shared" si="1"/>
         <v>119.31665823747248</v>
       </c>
       <c r="F16" s="3"/>
@@ -1555,15 +1559,15 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9">
+      <c r="A17" s="12"/>
+      <c r="B17" s="6">
         <v>3000</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="6">
         <v>463.59899999999999</v>
       </c>
-      <c r="D17" s="14">
-        <f>(2*(B17^3)/C17)/1000000</f>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
         <v>116.47997515093863</v>
       </c>
       <c r="F17" s="3"/>
@@ -1613,11 +1617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,97 +1662,97 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>600</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="10" t="e">
-        <f>(2*(B2^3)/C2)/1000000</f>
+      <c r="C2" s="5"/>
+      <c r="D2" s="7" t="e">
+        <f t="shared" ref="D2:D8" si="0">(2*(B2^3)/C2)/1000000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>4000</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="10" t="e">
+      <c r="H2" s="5"/>
+      <c r="I2" s="7" t="e">
         <f>(2*(G2^3)/H2)/1000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="4">
         <v>1000</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="13" t="e">
-        <f>(2*(B3^3)/C3)/1000000</f>
+      <c r="D3" s="8" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="4">
         <v>6000</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="13" t="e">
+      <c r="I3" s="8" t="e">
         <f>(2*(G3^3)/H3)/1000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="4">
         <v>1400</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="13" t="e">
-        <f>(2*(B4^3)/C4)/1000000</f>
+      <c r="D4" s="8" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="4">
         <v>8000</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="13" t="e">
+      <c r="I4" s="8" t="e">
         <f>(2*(G4^3)/H4)/1000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="4">
         <v>1800</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="13" t="e">
-        <f>(2*(B5^3)/C5)/1000000</f>
+      <c r="D5" s="8" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9">
+      <c r="F5" s="12"/>
+      <c r="G5" s="6">
         <v>10000</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="14" t="e">
+      <c r="H5" s="6"/>
+      <c r="I5" s="9" t="e">
         <f>(2*(G5^3)/H5)/1000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="4">
         <v>2200</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="13" t="e">
-        <f>(2*(B6^3)/C6)/1000000</f>
+      <c r="D6" s="8" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F6" s="3"/>
@@ -1757,13 +1761,13 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="4">
         <v>2600</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="13" t="e">
-        <f>(2*(B7^3)/C7)/1000000</f>
+      <c r="D7" s="8" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F7" s="3"/>
@@ -1772,13 +1776,13 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6">
         <v>3000</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="14" t="e">
-        <f>(2*(B8^3)/C8)/1000000</f>
+      <c r="C8" s="6"/>
+      <c r="D8" s="9" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F8" s="3"/>
@@ -1823,142 +1827,146 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>600</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.39300000000000002</v>
       </c>
-      <c r="D11" s="10">
-        <f>(2*(B11^3)/C11)/1000000</f>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11:D17" si="1">(2*(B11^3)/C11)/1000000</f>
         <v>1099.2366412213739</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>4000</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>164.512</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <f>(2*(G11^3)/H11)/1000000</f>
         <v>778.05874343512937</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="4">
         <v>1000</v>
       </c>
       <c r="C12" s="4">
         <v>2.83</v>
       </c>
-      <c r="D12" s="13">
-        <f>(2*(B12^3)/C12)/1000000</f>
+      <c r="D12" s="8">
+        <f t="shared" si="1"/>
         <v>706.71378091872782</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="4">
         <v>6000</v>
       </c>
       <c r="H12" s="4">
         <v>531.27300000000002</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="8">
         <f>(2*(G12^3)/H12)/1000000</f>
         <v>813.14126635458604</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="4">
         <v>1400</v>
       </c>
       <c r="C13" s="4">
         <v>7.4729999999999999</v>
       </c>
-      <c r="D13" s="13">
-        <f>(2*(B13^3)/C13)/1000000</f>
+      <c r="D13" s="8">
+        <f t="shared" si="1"/>
         <v>734.37709086043094</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="4">
         <v>8000</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="17"/>
+      <c r="H13" s="4">
+        <v>1024.972</v>
+      </c>
+      <c r="I13" s="8">
+        <f>(2*(G13^3)/H13)/1000000</f>
+        <v>999.0516814117849</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="4">
         <v>1800</v>
       </c>
       <c r="C14" s="4">
         <v>19.247</v>
       </c>
-      <c r="D14" s="13">
-        <f>(2*(B14^3)/C14)/1000000</f>
+      <c r="D14" s="8">
+        <f t="shared" si="1"/>
         <v>606.01652205538528</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="9">
+      <c r="F14" s="12"/>
+      <c r="G14" s="6">
         <v>10000</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="19"/>
+      <c r="H14" s="6">
+        <v>1762.0840000000001</v>
+      </c>
+      <c r="I14" s="9">
+        <f>(2*(G14^3)/H14)/1000000</f>
+        <v>1135.0196698908792</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="4">
         <v>2200</v>
       </c>
       <c r="C15" s="4">
         <v>27.372</v>
       </c>
-      <c r="D15" s="13">
-        <f>(2*(B15^3)/C15)/1000000</f>
+      <c r="D15" s="8">
+        <f t="shared" si="1"/>
         <v>778.02133567148917</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="4">
         <v>2600</v>
       </c>
       <c r="C16" s="4">
         <v>45.738999999999997</v>
       </c>
-      <c r="D16" s="13">
-        <f>(2*(B16^3)/C16)/1000000</f>
+      <c r="D16" s="8">
+        <f t="shared" si="1"/>
         <v>768.53451102997451</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9">
+      <c r="A17" s="12"/>
+      <c r="B17" s="6">
         <v>3000</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="6">
         <v>69.876000000000005</v>
       </c>
-      <c r="D17" s="14">
-        <f>(2*(B17^3)/C17)/1000000</f>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
         <v>772.79752704791338</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
+  <mergeCells count="4">
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="F2:F5"/>
@@ -1966,6 +1974,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
c++ code, for 10000 test
</commit_message>
<xml_diff>
--- a/Lab1/docs/Statistics.xlsx
+++ b/Lab1/docs/Statistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise 1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Exercise 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -357,32 +358,68 @@
             <c:v>C/C++</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$B$2:$B$8</c:f>
+              <c:f>'Exercise 1'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -412,30 +449,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$D$2:$D$8</c:f>
+              <c:f>'Exercise 1'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1380.1916932907347</c:v>
+                  <c:v>304.43974630021143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1041.1244143675169</c:v>
+                  <c:v>255.9836170485089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1017.992951214988</c:v>
+                  <c:v>248.22470487131935</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>977.12993214375467</c:v>
+                  <c:v>236.05601878086296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1013.9021138830699</c:v>
+                  <c:v>225.42128884748919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>998.52289512555387</c:v>
+                  <c:v>185.79379383611962</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>997.89333629005444</c:v>
+                  <c:v>188.22807665762704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -449,32 +486,68 @@
             <c:v>Java</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$B$11:$B$17</c:f>
+              <c:f>'Exercise 1'!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -504,30 +577,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$D$11:$D$17</c:f>
+              <c:f>'Exercise 1'!$D$11:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1099.2366412213739</c:v>
+                  <c:v>209.60698689956331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>706.71378091872782</c:v>
+                  <c:v>156.04275571506594</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>734.37709086043094</c:v>
+                  <c:v>148.03625377643505</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>606.01652205538528</c:v>
+                  <c:v>134.91411717078248</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>778.02133567148917</c:v>
+                  <c:v>121.22799127905321</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>768.53451102997451</c:v>
+                  <c:v>119.31665823747248</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>772.79752704791338</c:v>
+                  <c:v>116.47997515093863</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -542,11 +615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-401055952"/>
-        <c:axId val="-401055408"/>
+        <c:axId val="-523104784"/>
+        <c:axId val="-523104176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-401055952"/>
+        <c:axId val="-523104784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,9 +629,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -573,11 +646,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -585,7 +657,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>n</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -603,11 +678,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -627,12 +701,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -643,9 +715,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -656,12 +727,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-401055408"/>
+        <c:crossAx val="-523104176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-401055408"/>
+        <c:axId val="-523104176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,9 +742,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -688,11 +759,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -728,11 +798,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -752,12 +821,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -768,9 +835,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -781,7 +847,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-401055952"/>
+        <c:crossAx val="-523104784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -811,9 +877,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -830,17 +895,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -889,67 +965,121 @@
             <c:v>C/C++</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$G$2:$G$5</c:f>
+              <c:f>'Exercise 2'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4000</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8000</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$I$2:$I$5</c:f>
+              <c:f>'Exercise 2'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>998.59572476205324</c:v>
+                  <c:v>1380.1916932907347</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1144.7044171811654</c:v>
+                  <c:v>1041.1244143675169</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1132.5153564216052</c:v>
+                  <c:v>1017.992951214988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>977.12993214375467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1013.9021138830699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>998.52289512555387</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>997.89333629005444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -963,67 +1093,121 @@
             <c:v>Java</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$G$11:$G$14</c:f>
+              <c:f>'Exercise 2'!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4000</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8000</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Exercise 2'!$I$11:$I$14</c:f>
+              <c:f>'Exercise 2'!$D$11:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>778.05874343512937</c:v>
+                  <c:v>1099.2366412213739</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>813.14126635458604</c:v>
+                  <c:v>706.71378091872782</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>999.0516814117849</c:v>
+                  <c:v>734.37709086043094</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1135.0196698908792</c:v>
+                  <c:v>606.01652205538528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>778.02133567148917</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>768.53451102997451</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>772.79752704791338</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,11 +1222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-401059216"/>
-        <c:axId val="-401054320"/>
+        <c:axId val="-523109648"/>
+        <c:axId val="-523109040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-401059216"/>
+        <c:axId val="-523109648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,9 +1236,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1062,6 +1246,60 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1070,12 +1308,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1086,9 +1322,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1099,12 +1334,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-401054320"/>
+        <c:crossAx val="-523109040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-401054320"/>
+        <c:axId val="-523109040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,9 +1349,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1124,6 +1359,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Capacidade</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.27164698162729661"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1132,12 +1428,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1148,9 +1442,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1161,7 +1454,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-401059216"/>
+        <c:crossAx val="-523109648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1191,9 +1484,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1210,17 +1502,592 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>C/C++</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exercise 2'!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exercise 2'!$I$2:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>998.59572476205324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1144.7044171811654</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1132.5153564216052</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Java</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exercise 2'!$G$11:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exercise 2'!$I$11:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>778.05874343512937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>813.14126635458604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>999.0516814117849</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1135.0196698908792</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-523031296"/>
+        <c:axId val="-523018528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-523031296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-523018528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-523018528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Capacidade</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-523031296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1322,63 +2189,107 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1387,9 +2298,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1408,14 +2318,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1424,20 +2326,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1446,48 +2348,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1497,27 +2361,63 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPointWireframe>
   <cs:dataTable>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1536,18 +2436,62 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1557,194 +2501,154 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:seriesLine>
   <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1760,7 +2664,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1769,9 +2673,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1787,36 +2690,32 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1828,73 +2727,71 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1903,9 +2800,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1924,14 +2820,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1940,20 +2828,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1962,48 +2850,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2013,27 +2863,63 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPointWireframe>
   <cs:dataTable>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2052,18 +2938,62 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2073,194 +3003,154 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:seriesLine>
   <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2276,7 +3166,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2285,56 +3175,553 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2344,12 +3731,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2358,10 +3739,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800099</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2419351" cy="461963"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -2373,7 +3754,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6448424" y="319087"/>
+              <a:off x="10067924" y="328612"/>
               <a:ext cx="2419351" cy="461963"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2561,7 +3942,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6448424" y="319087"/>
+              <a:off x="10067924" y="328612"/>
               <a:ext cx="2419351" cy="461963"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2607,16 +3988,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2625,7 +4006,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6581775" y="1000126"/>
+          <a:off x="10258425" y="1123951"/>
           <a:ext cx="2085975" cy="1076324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2715,6 +4096,38 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3116,15 +4529,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1400175</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>1343025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3413,8 +4826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,8 +5119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>